<commit_message>
HW 7 Lacking write up
</commit_message>
<xml_diff>
--- a/HW7_DiscreteOptimization/Prb2.xlsx
+++ b/HW7_DiscreteOptimization/Prb2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\child\Documents\Projects\Optimization\HW7_DiscreteOptimization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchild25\Documents\Projects\Optimization\HW7_DiscreteOptimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1640ED-835A-4DA4-8338-35F6D38A8E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9D559E-6A8A-4067-AA96-0BC48D7520A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{E893D32F-30B7-4F66-BA62-D4BFF2B249EB}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="12225" xr2:uid="{E893D32F-30B7-4F66-BA62-D4BFF2B249EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Node</t>
   </si>
@@ -99,13 +88,22 @@
   </si>
   <si>
     <t>Na</t>
+  </si>
+  <si>
+    <t>K or L</t>
+  </si>
+  <si>
+    <t>Note: Both had the same cost</t>
+  </si>
+  <si>
+    <t>F or G</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,23 +164,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>450850</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>66425</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>329950</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{867C9363-0869-E94B-E76C-3B5DC67E0A88}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0532A246-C1B2-4FC1-8C39-C2183A530337}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -198,8 +196,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4718050" y="133350"/>
-          <a:ext cx="5101975" cy="3848100"/>
+          <a:off x="28575" y="3629025"/>
+          <a:ext cx="5787775" cy="3952875"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -528,15 +526,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{005825B8-BE36-4BE3-9C0D-DF8C52A876D2}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,57 +545,130 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <f>MIN(9+B7,3+B8,10+B9,7+B10)</f>
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <f>19</f>
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <f>MIN(10+B7,5+B8,3+B9,7+B10)</f>
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <f>MIN(5+B11,8+B12,1+B13)</f>
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <f>MIN(5+B11,8+B12,7+B13)</f>
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <f>MIN(4+B11,5+B12,7+B13)</f>
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <f>MIN(4+B11,5+B12,9+B13)</f>
+        <v>16</v>
+      </c>
+      <c r="C10" t="str">
+        <f>INDEX(A11:A13, MATCH(B10, CHOOSE({1,2,3,4},4+B11,5+B12,9+B13), 0))</f>
+        <v>K</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <f>MIN(9+B14,9+B15,8+B16,10+B17)</f>
+        <v>16</v>
+      </c>
+      <c r="C11" t="str">
+        <f>INDEX(A14:A17, MATCH(B11, CHOOSE({1,2,3,4},9+B14,9+B15,8+B16,10+B17), 0))</f>
+        <v xml:space="preserve">N </v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -605,11 +676,12 @@
         <f>MIN(4+B14,10+B15,6+B16,4+B17)</f>
         <v>11</v>
       </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C12" t="str">
+        <f>INDEX(A14:A17, MATCH(B12, CHOOSE({1,2,3,4}, 4+B14,10+B15,6+B16,4+B17), 0))</f>
+        <v>P</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -621,7 +693,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="15">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -632,7 +704,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="15">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -643,7 +715,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="15">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -654,7 +726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="15">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -665,7 +737,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="15">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
HW7 done, cfd update
</commit_message>
<xml_diff>
--- a/HW7_DiscreteOptimization/Prb2.xlsx
+++ b/HW7_DiscreteOptimization/Prb2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchild25\Documents\Projects\Optimization\HW7_DiscreteOptimization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\child\Documents\Projects\Optimization\HW7_DiscreteOptimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9D559E-6A8A-4067-AA96-0BC48D7520A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131304F2-606B-4DAC-BDFA-647D076C4723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="12225" xr2:uid="{E893D32F-30B7-4F66-BA62-D4BFF2B249EB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{E893D32F-30B7-4F66-BA62-D4BFF2B249EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Node</t>
   </si>
@@ -91,9 +102,6 @@
   </si>
   <si>
     <t>K or L</t>
-  </si>
-  <si>
-    <t>Note: Both had the same cost</t>
   </si>
   <si>
     <t>F or G</t>
@@ -103,7 +111,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,15 +534,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{005825B8-BE36-4BE3-9C0D-DF8C52A876D2}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -556,7 +564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -567,7 +575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -576,10 +584,10 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -591,7 +599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -603,7 +611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -615,7 +623,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -627,7 +635,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -638,11 +646,8 @@
       <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -655,7 +660,7 @@
         <v>K</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -668,7 +673,7 @@
         <v xml:space="preserve">N </v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -681,7 +686,7 @@
         <v>P</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -693,7 +698,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -704,7 +709,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -715,7 +720,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -726,7 +731,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -737,7 +742,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>

</xml_diff>